<commit_message>
V3_Correção Data de emissão
</commit_message>
<xml_diff>
--- a/Arquivo/saida_competencia_test.xlsx
+++ b/Arquivo/saida_competencia_test.xlsx
@@ -85,7 +85,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
@@ -94,11 +94,12 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -568,8 +569,10 @@
           <t>202200000000001</t>
         </is>
       </c>
-      <c r="B2" s="4" t="n">
-        <v>3012022</v>
+      <c r="B2" s="4" t="inlineStr">
+        <is>
+          <t>03/01/2022</t>
+        </is>
       </c>
       <c r="C2" s="5" t="inlineStr">
         <is>
@@ -596,7 +599,7 @@
           <t>44.112,20</t>
         </is>
       </c>
-      <c r="H2" s="4" t="n">
+      <c r="H2" s="6" t="n">
         <v>44112.2</v>
       </c>
       <c r="I2" s="3" t="inlineStr">
@@ -604,10 +607,10 @@
           <t>3,00 %</t>
         </is>
       </c>
-      <c r="J2" s="4" t="n">
+      <c r="J2" s="6" t="n">
         <v>1323.37</v>
       </c>
-      <c r="K2" s="4" t="n">
+      <c r="K2" s="6" t="n">
         <v>0</v>
       </c>
       <c r="L2" s="3" t="inlineStr">
@@ -632,8 +635,10 @@
           <t>202200000000002</t>
         </is>
       </c>
-      <c r="B3" s="4" t="n">
-        <v>3012022</v>
+      <c r="B3" s="4" t="inlineStr">
+        <is>
+          <t>03/01/2022</t>
+        </is>
       </c>
       <c r="C3" s="5" t="inlineStr">
         <is>
@@ -660,7 +665,7 @@
           <t>20,00</t>
         </is>
       </c>
-      <c r="H3" s="4" t="n">
+      <c r="H3" s="6" t="n">
         <v>20</v>
       </c>
       <c r="I3" s="3" t="inlineStr">
@@ -668,10 +673,10 @@
           <t>3,00 %</t>
         </is>
       </c>
-      <c r="J3" s="4" t="n">
+      <c r="J3" s="6" t="n">
         <v>0.6</v>
       </c>
-      <c r="K3" s="4" t="n">
+      <c r="K3" s="6" t="n">
         <v>0</v>
       </c>
       <c r="L3" s="3" t="inlineStr">
@@ -696,8 +701,10 @@
           <t>202200000000003</t>
         </is>
       </c>
-      <c r="B4" s="4" t="n">
-        <v>3012022</v>
+      <c r="B4" s="4" t="inlineStr">
+        <is>
+          <t>03/01/2022</t>
+        </is>
       </c>
       <c r="C4" s="5" t="inlineStr">
         <is>
@@ -724,7 +731,7 @@
           <t>20,00</t>
         </is>
       </c>
-      <c r="H4" s="4" t="n">
+      <c r="H4" s="6" t="n">
         <v>20</v>
       </c>
       <c r="I4" s="3" t="inlineStr">
@@ -732,10 +739,10 @@
           <t>3,00 %</t>
         </is>
       </c>
-      <c r="J4" s="4" t="n">
+      <c r="J4" s="6" t="n">
         <v>0.6</v>
       </c>
-      <c r="K4" s="4" t="n">
+      <c r="K4" s="6" t="n">
         <v>0</v>
       </c>
       <c r="L4" s="3" t="inlineStr">
@@ -760,8 +767,10 @@
           <t>202200000000004</t>
         </is>
       </c>
-      <c r="B5" s="4" t="n">
-        <v>3012022</v>
+      <c r="B5" s="4" t="inlineStr">
+        <is>
+          <t>03/01/2022</t>
+        </is>
       </c>
       <c r="C5" s="5" t="inlineStr">
         <is>
@@ -788,7 +797,7 @@
           <t>350,00</t>
         </is>
       </c>
-      <c r="H5" s="4" t="n">
+      <c r="H5" s="6" t="n">
         <v>350</v>
       </c>
       <c r="I5" s="3" t="inlineStr">
@@ -796,10 +805,10 @@
           <t>3,00 %</t>
         </is>
       </c>
-      <c r="J5" s="4" t="n">
+      <c r="J5" s="6" t="n">
         <v>10.5</v>
       </c>
-      <c r="K5" s="4" t="n">
+      <c r="K5" s="6" t="n">
         <v>0</v>
       </c>
       <c r="L5" s="3" t="inlineStr">
@@ -824,8 +833,10 @@
           <t>202200000000005</t>
         </is>
       </c>
-      <c r="B6" s="4" t="n">
-        <v>3012022</v>
+      <c r="B6" s="4" t="inlineStr">
+        <is>
+          <t>03/01/2022</t>
+        </is>
       </c>
       <c r="C6" s="5" t="inlineStr">
         <is>
@@ -852,7 +863,7 @@
           <t>120,00</t>
         </is>
       </c>
-      <c r="H6" s="4" t="n">
+      <c r="H6" s="6" t="n">
         <v>120</v>
       </c>
       <c r="I6" s="3" t="inlineStr">
@@ -860,10 +871,10 @@
           <t>3,00 %</t>
         </is>
       </c>
-      <c r="J6" s="4" t="n">
+      <c r="J6" s="6" t="n">
         <v>3.6</v>
       </c>
-      <c r="K6" s="4" t="n">
+      <c r="K6" s="6" t="n">
         <v>0</v>
       </c>
       <c r="L6" s="3" t="inlineStr">
@@ -888,8 +899,10 @@
           <t>202200000000006</t>
         </is>
       </c>
-      <c r="B7" s="4" t="n">
-        <v>3012022</v>
+      <c r="B7" s="4" t="inlineStr">
+        <is>
+          <t>03/01/2022</t>
+        </is>
       </c>
       <c r="C7" s="5" t="inlineStr">
         <is>
@@ -916,7 +929,7 @@
           <t>20,00</t>
         </is>
       </c>
-      <c r="H7" s="4" t="n">
+      <c r="H7" s="6" t="n">
         <v>20</v>
       </c>
       <c r="I7" s="3" t="inlineStr">
@@ -924,10 +937,10 @@
           <t>3,00 %</t>
         </is>
       </c>
-      <c r="J7" s="4" t="n">
+      <c r="J7" s="6" t="n">
         <v>0.6</v>
       </c>
-      <c r="K7" s="4" t="n">
+      <c r="K7" s="6" t="n">
         <v>0</v>
       </c>
       <c r="L7" s="3" t="inlineStr">
@@ -952,8 +965,10 @@
           <t>202200000000007</t>
         </is>
       </c>
-      <c r="B8" s="4" t="n">
-        <v>3012022</v>
+      <c r="B8" s="4" t="inlineStr">
+        <is>
+          <t>03/01/2022</t>
+        </is>
       </c>
       <c r="C8" s="5" t="inlineStr">
         <is>
@@ -980,7 +995,7 @@
           <t>16,89</t>
         </is>
       </c>
-      <c r="H8" s="4" t="n">
+      <c r="H8" s="6" t="n">
         <v>16.89</v>
       </c>
       <c r="I8" s="3" t="inlineStr">
@@ -988,10 +1003,10 @@
           <t>3,00 %</t>
         </is>
       </c>
-      <c r="J8" s="4" t="n">
+      <c r="J8" s="6" t="n">
         <v>0.51</v>
       </c>
-      <c r="K8" s="4" t="n">
+      <c r="K8" s="6" t="n">
         <v>0</v>
       </c>
       <c r="L8" s="3" t="inlineStr">
@@ -1016,8 +1031,10 @@
           <t>202200000000008</t>
         </is>
       </c>
-      <c r="B9" s="4" t="n">
-        <v>3012022</v>
+      <c r="B9" s="4" t="inlineStr">
+        <is>
+          <t>03/01/2022</t>
+        </is>
       </c>
       <c r="C9" s="5" t="inlineStr">
         <is>
@@ -1044,7 +1061,7 @@
           <t>350,00</t>
         </is>
       </c>
-      <c r="H9" s="4" t="n">
+      <c r="H9" s="6" t="n">
         <v>350</v>
       </c>
       <c r="I9" s="3" t="inlineStr">
@@ -1052,10 +1069,10 @@
           <t>3,00 %</t>
         </is>
       </c>
-      <c r="J9" s="4" t="n">
+      <c r="J9" s="6" t="n">
         <v>10.5</v>
       </c>
-      <c r="K9" s="4" t="n">
+      <c r="K9" s="6" t="n">
         <v>0</v>
       </c>
       <c r="L9" s="3" t="inlineStr">
@@ -1080,8 +1097,10 @@
           <t>202200000000009</t>
         </is>
       </c>
-      <c r="B10" s="4" t="n">
-        <v>3012022</v>
+      <c r="B10" s="4" t="inlineStr">
+        <is>
+          <t>03/01/2022</t>
+        </is>
       </c>
       <c r="C10" s="5" t="inlineStr">
         <is>
@@ -1108,7 +1127,7 @@
           <t>7.500,00</t>
         </is>
       </c>
-      <c r="H10" s="4" t="n">
+      <c r="H10" s="6" t="n">
         <v>7500</v>
       </c>
       <c r="I10" s="3" t="inlineStr">
@@ -1116,10 +1135,10 @@
           <t>3,00 %</t>
         </is>
       </c>
-      <c r="J10" s="4" t="n">
+      <c r="J10" s="6" t="n">
         <v>225</v>
       </c>
-      <c r="K10" s="4" t="n">
+      <c r="K10" s="6" t="n">
         <v>0</v>
       </c>
       <c r="L10" s="3" t="inlineStr">
@@ -1144,8 +1163,10 @@
           <t>202200000000010</t>
         </is>
       </c>
-      <c r="B11" s="4" t="n">
-        <v>3012022</v>
+      <c r="B11" s="4" t="inlineStr">
+        <is>
+          <t>03/01/2022</t>
+        </is>
       </c>
       <c r="C11" s="5" t="inlineStr">
         <is>
@@ -1172,7 +1193,7 @@
           <t>470,00</t>
         </is>
       </c>
-      <c r="H11" s="4" t="n">
+      <c r="H11" s="6" t="n">
         <v>470</v>
       </c>
       <c r="I11" s="3" t="inlineStr">
@@ -1180,10 +1201,10 @@
           <t>3,00 %</t>
         </is>
       </c>
-      <c r="J11" s="4" t="n">
+      <c r="J11" s="6" t="n">
         <v>14.1</v>
       </c>
-      <c r="K11" s="4" t="n">
+      <c r="K11" s="6" t="n">
         <v>0</v>
       </c>
       <c r="L11" s="3" t="inlineStr">
@@ -1208,8 +1229,10 @@
           <t>202200000000011</t>
         </is>
       </c>
-      <c r="B12" s="4" t="n">
-        <v>3012022</v>
+      <c r="B12" s="4" t="inlineStr">
+        <is>
+          <t>03/01/2022</t>
+        </is>
       </c>
       <c r="C12" s="5" t="inlineStr">
         <is>
@@ -1236,7 +1259,7 @@
           <t>20,00</t>
         </is>
       </c>
-      <c r="H12" s="4" t="n">
+      <c r="H12" s="6" t="n">
         <v>20</v>
       </c>
       <c r="I12" s="3" t="inlineStr">
@@ -1244,10 +1267,10 @@
           <t>3,00 %</t>
         </is>
       </c>
-      <c r="J12" s="4" t="n">
+      <c r="J12" s="6" t="n">
         <v>0.6</v>
       </c>
-      <c r="K12" s="4" t="n">
+      <c r="K12" s="6" t="n">
         <v>0</v>
       </c>
       <c r="L12" s="3" t="inlineStr">
@@ -1272,8 +1295,10 @@
           <t>202200000000012</t>
         </is>
       </c>
-      <c r="B13" s="4" t="n">
-        <v>4012022</v>
+      <c r="B13" s="4" t="inlineStr">
+        <is>
+          <t>04/01/2022</t>
+        </is>
       </c>
       <c r="C13" s="5" t="inlineStr">
         <is>
@@ -1300,7 +1325,7 @@
           <t>16,89</t>
         </is>
       </c>
-      <c r="H13" s="4" t="n">
+      <c r="H13" s="6" t="n">
         <v>16.89</v>
       </c>
       <c r="I13" s="3" t="inlineStr">
@@ -1308,10 +1333,10 @@
           <t>3,00 %</t>
         </is>
       </c>
-      <c r="J13" s="4" t="n">
+      <c r="J13" s="6" t="n">
         <v>0.51</v>
       </c>
-      <c r="K13" s="4" t="n">
+      <c r="K13" s="6" t="n">
         <v>0</v>
       </c>
       <c r="L13" s="3" t="inlineStr">
@@ -1336,8 +1361,10 @@
           <t>202200000000013</t>
         </is>
       </c>
-      <c r="B14" s="4" t="n">
-        <v>4012022</v>
+      <c r="B14" s="4" t="inlineStr">
+        <is>
+          <t>04/01/2022</t>
+        </is>
       </c>
       <c r="C14" s="5" t="inlineStr">
         <is>
@@ -1364,7 +1391,7 @@
           <t>920,00</t>
         </is>
       </c>
-      <c r="H14" s="4" t="n">
+      <c r="H14" s="6" t="n">
         <v>920</v>
       </c>
       <c r="I14" s="3" t="inlineStr">
@@ -1372,10 +1399,10 @@
           <t>3,00 %</t>
         </is>
       </c>
-      <c r="J14" s="4" t="n">
+      <c r="J14" s="6" t="n">
         <v>27.6</v>
       </c>
-      <c r="K14" s="4" t="n">
+      <c r="K14" s="6" t="n">
         <v>0</v>
       </c>
       <c r="L14" s="3" t="inlineStr">
@@ -1400,8 +1427,10 @@
           <t>202200000000014</t>
         </is>
       </c>
-      <c r="B15" s="4" t="n">
-        <v>4012022</v>
+      <c r="B15" s="4" t="inlineStr">
+        <is>
+          <t>04/01/2022</t>
+        </is>
       </c>
       <c r="C15" s="5" t="inlineStr">
         <is>
@@ -1428,7 +1457,7 @@
           <t>470,00</t>
         </is>
       </c>
-      <c r="H15" s="4" t="n">
+      <c r="H15" s="6" t="n">
         <v>470</v>
       </c>
       <c r="I15" s="3" t="inlineStr">
@@ -1436,10 +1465,10 @@
           <t>3,00 %</t>
         </is>
       </c>
-      <c r="J15" s="4" t="n">
+      <c r="J15" s="6" t="n">
         <v>14.1</v>
       </c>
-      <c r="K15" s="4" t="n">
+      <c r="K15" s="6" t="n">
         <v>0</v>
       </c>
       <c r="L15" s="3" t="inlineStr">
@@ -1464,8 +1493,10 @@
           <t>202200000000015</t>
         </is>
       </c>
-      <c r="B16" s="4" t="n">
-        <v>4012022</v>
+      <c r="B16" s="4" t="inlineStr">
+        <is>
+          <t>04/01/2022</t>
+        </is>
       </c>
       <c r="C16" s="5" t="inlineStr">
         <is>
@@ -1492,7 +1523,7 @@
           <t>470,00</t>
         </is>
       </c>
-      <c r="H16" s="4" t="n">
+      <c r="H16" s="6" t="n">
         <v>470</v>
       </c>
       <c r="I16" s="3" t="inlineStr">
@@ -1500,10 +1531,10 @@
           <t>3,00 %</t>
         </is>
       </c>
-      <c r="J16" s="4" t="n">
+      <c r="J16" s="6" t="n">
         <v>14.1</v>
       </c>
-      <c r="K16" s="4" t="n">
+      <c r="K16" s="6" t="n">
         <v>0</v>
       </c>
       <c r="L16" s="3" t="inlineStr">
@@ -1528,8 +1559,10 @@
           <t>202200000000016</t>
         </is>
       </c>
-      <c r="B17" s="4" t="n">
-        <v>4012022</v>
+      <c r="B17" s="4" t="inlineStr">
+        <is>
+          <t>04/01/2022</t>
+        </is>
       </c>
       <c r="C17" s="5" t="inlineStr">
         <is>
@@ -1556,7 +1589,7 @@
           <t>1.040,00</t>
         </is>
       </c>
-      <c r="H17" s="4" t="n">
+      <c r="H17" s="6" t="n">
         <v>1040</v>
       </c>
       <c r="I17" s="3" t="inlineStr">
@@ -1564,10 +1597,10 @@
           <t>3,00 %</t>
         </is>
       </c>
-      <c r="J17" s="4" t="n">
+      <c r="J17" s="6" t="n">
         <v>31.2</v>
       </c>
-      <c r="K17" s="4" t="n">
+      <c r="K17" s="6" t="n">
         <v>0</v>
       </c>
       <c r="L17" s="3" t="inlineStr">
@@ -1592,8 +1625,10 @@
           <t>202200000000017</t>
         </is>
       </c>
-      <c r="B18" s="4" t="n">
-        <v>4012022</v>
+      <c r="B18" s="4" t="inlineStr">
+        <is>
+          <t>04/01/2022</t>
+        </is>
       </c>
       <c r="C18" s="5" t="inlineStr">
         <is>
@@ -1620,7 +1655,7 @@
           <t>350,00</t>
         </is>
       </c>
-      <c r="H18" s="4" t="n">
+      <c r="H18" s="6" t="n">
         <v>350</v>
       </c>
       <c r="I18" s="3" t="inlineStr">
@@ -1628,10 +1663,10 @@
           <t>3,00 %</t>
         </is>
       </c>
-      <c r="J18" s="4" t="n">
+      <c r="J18" s="6" t="n">
         <v>10.5</v>
       </c>
-      <c r="K18" s="4" t="n">
+      <c r="K18" s="6" t="n">
         <v>0</v>
       </c>
       <c r="L18" s="3" t="inlineStr">
@@ -1656,8 +1691,10 @@
           <t>202200000000018</t>
         </is>
       </c>
-      <c r="B19" s="4" t="n">
-        <v>4012022</v>
+      <c r="B19" s="4" t="inlineStr">
+        <is>
+          <t>04/01/2022</t>
+        </is>
       </c>
       <c r="C19" s="5" t="inlineStr">
         <is>
@@ -1684,7 +1721,7 @@
           <t>20,00</t>
         </is>
       </c>
-      <c r="H19" s="4" t="n">
+      <c r="H19" s="6" t="n">
         <v>20</v>
       </c>
       <c r="I19" s="3" t="inlineStr">
@@ -1692,10 +1729,10 @@
           <t>3,00 %</t>
         </is>
       </c>
-      <c r="J19" s="4" t="n">
+      <c r="J19" s="6" t="n">
         <v>0.6</v>
       </c>
-      <c r="K19" s="4" t="n">
+      <c r="K19" s="6" t="n">
         <v>0</v>
       </c>
       <c r="L19" s="3" t="inlineStr">
@@ -1720,8 +1757,10 @@
           <t>202200000000019</t>
         </is>
       </c>
-      <c r="B20" s="4" t="n">
-        <v>4012022</v>
+      <c r="B20" s="4" t="inlineStr">
+        <is>
+          <t>04/01/2022</t>
+        </is>
       </c>
       <c r="C20" s="5" t="inlineStr">
         <is>
@@ -1748,7 +1787,7 @@
           <t>350,00</t>
         </is>
       </c>
-      <c r="H20" s="4" t="n">
+      <c r="H20" s="6" t="n">
         <v>350</v>
       </c>
       <c r="I20" s="3" t="inlineStr">
@@ -1756,10 +1795,10 @@
           <t>3,00 %</t>
         </is>
       </c>
-      <c r="J20" s="4" t="n">
+      <c r="J20" s="6" t="n">
         <v>10.5</v>
       </c>
-      <c r="K20" s="4" t="n">
+      <c r="K20" s="6" t="n">
         <v>0</v>
       </c>
       <c r="L20" s="3" t="inlineStr">
@@ -1784,8 +1823,10 @@
           <t>202200000000020</t>
         </is>
       </c>
-      <c r="B21" s="4" t="n">
-        <v>4012022</v>
+      <c r="B21" s="4" t="inlineStr">
+        <is>
+          <t>04/01/2022</t>
+        </is>
       </c>
       <c r="C21" s="5" t="inlineStr">
         <is>
@@ -1812,7 +1853,7 @@
           <t>20,00</t>
         </is>
       </c>
-      <c r="H21" s="4" t="n">
+      <c r="H21" s="6" t="n">
         <v>20</v>
       </c>
       <c r="I21" s="3" t="inlineStr">
@@ -1820,10 +1861,10 @@
           <t>3,00 %</t>
         </is>
       </c>
-      <c r="J21" s="4" t="n">
+      <c r="J21" s="6" t="n">
         <v>0.6</v>
       </c>
-      <c r="K21" s="4" t="n">
+      <c r="K21" s="6" t="n">
         <v>0</v>
       </c>
       <c r="L21" s="3" t="inlineStr">
@@ -1848,8 +1889,10 @@
           <t>202200000000021</t>
         </is>
       </c>
-      <c r="B22" s="4" t="n">
-        <v>4012022</v>
+      <c r="B22" s="4" t="inlineStr">
+        <is>
+          <t>04/01/2022</t>
+        </is>
       </c>
       <c r="C22" s="5" t="inlineStr">
         <is>
@@ -1876,7 +1919,7 @@
           <t>470,00</t>
         </is>
       </c>
-      <c r="H22" s="4" t="n">
+      <c r="H22" s="6" t="n">
         <v>470</v>
       </c>
       <c r="I22" s="3" t="inlineStr">
@@ -1884,10 +1927,10 @@
           <t>3,00 %</t>
         </is>
       </c>
-      <c r="J22" s="4" t="n">
+      <c r="J22" s="6" t="n">
         <v>14.1</v>
       </c>
-      <c r="K22" s="4" t="n">
+      <c r="K22" s="6" t="n">
         <v>0</v>
       </c>
       <c r="L22" s="3" t="inlineStr">
@@ -1912,8 +1955,10 @@
           <t>202200000000022</t>
         </is>
       </c>
-      <c r="B23" s="4" t="n">
-        <v>4012022</v>
+      <c r="B23" s="4" t="inlineStr">
+        <is>
+          <t>04/01/2022</t>
+        </is>
       </c>
       <c r="C23" s="5" t="inlineStr">
         <is>
@@ -1940,7 +1985,7 @@
           <t>470,00</t>
         </is>
       </c>
-      <c r="H23" s="4" t="n">
+      <c r="H23" s="6" t="n">
         <v>470</v>
       </c>
       <c r="I23" s="3" t="inlineStr">
@@ -1948,10 +1993,10 @@
           <t>3,00 %</t>
         </is>
       </c>
-      <c r="J23" s="4" t="n">
+      <c r="J23" s="6" t="n">
         <v>14.1</v>
       </c>
-      <c r="K23" s="4" t="n">
+      <c r="K23" s="6" t="n">
         <v>0</v>
       </c>
       <c r="L23" s="3" t="inlineStr">
@@ -1976,8 +2021,10 @@
           <t>202200000000023</t>
         </is>
       </c>
-      <c r="B24" s="4" t="n">
-        <v>4012022</v>
+      <c r="B24" s="4" t="inlineStr">
+        <is>
+          <t>04/01/2022</t>
+        </is>
       </c>
       <c r="C24" s="5" t="inlineStr">
         <is>
@@ -2004,7 +2051,7 @@
           <t>2.200,00</t>
         </is>
       </c>
-      <c r="H24" s="4" t="n">
+      <c r="H24" s="6" t="n">
         <v>2200</v>
       </c>
       <c r="I24" s="3" t="inlineStr">
@@ -2012,10 +2059,10 @@
           <t>3,00 %</t>
         </is>
       </c>
-      <c r="J24" s="4" t="n">
+      <c r="J24" s="6" t="n">
         <v>66</v>
       </c>
-      <c r="K24" s="4" t="n">
+      <c r="K24" s="6" t="n">
         <v>0</v>
       </c>
       <c r="L24" s="3" t="inlineStr">
@@ -2040,8 +2087,10 @@
           <t>202200000000024</t>
         </is>
       </c>
-      <c r="B25" s="4" t="n">
-        <v>4012022</v>
+      <c r="B25" s="4" t="inlineStr">
+        <is>
+          <t>04/01/2022</t>
+        </is>
       </c>
       <c r="C25" s="5" t="inlineStr">
         <is>
@@ -2068,7 +2117,7 @@
           <t>20,00</t>
         </is>
       </c>
-      <c r="H25" s="4" t="n">
+      <c r="H25" s="6" t="n">
         <v>20</v>
       </c>
       <c r="I25" s="3" t="inlineStr">
@@ -2076,10 +2125,10 @@
           <t>3,00 %</t>
         </is>
       </c>
-      <c r="J25" s="4" t="n">
+      <c r="J25" s="6" t="n">
         <v>0.6</v>
       </c>
-      <c r="K25" s="4" t="n">
+      <c r="K25" s="6" t="n">
         <v>0</v>
       </c>
       <c r="L25" s="3" t="inlineStr">
@@ -2104,8 +2153,10 @@
           <t>202200000000025</t>
         </is>
       </c>
-      <c r="B26" s="4" t="n">
-        <v>4012022</v>
+      <c r="B26" s="4" t="inlineStr">
+        <is>
+          <t>04/01/2022</t>
+        </is>
       </c>
       <c r="C26" s="5" t="inlineStr">
         <is>
@@ -2132,7 +2183,7 @@
           <t>350,00</t>
         </is>
       </c>
-      <c r="H26" s="4" t="n">
+      <c r="H26" s="6" t="n">
         <v>350</v>
       </c>
       <c r="I26" s="3" t="inlineStr">
@@ -2140,10 +2191,10 @@
           <t>3,00 %</t>
         </is>
       </c>
-      <c r="J26" s="4" t="n">
+      <c r="J26" s="6" t="n">
         <v>10.5</v>
       </c>
-      <c r="K26" s="4" t="n">
+      <c r="K26" s="6" t="n">
         <v>0</v>
       </c>
       <c r="L26" s="3" t="inlineStr">
@@ -2168,8 +2219,10 @@
           <t>202200000000026</t>
         </is>
       </c>
-      <c r="B27" s="4" t="n">
-        <v>4012022</v>
+      <c r="B27" s="4" t="inlineStr">
+        <is>
+          <t>04/01/2022</t>
+        </is>
       </c>
       <c r="C27" s="5" t="inlineStr">
         <is>
@@ -2196,7 +2249,7 @@
           <t>64,69</t>
         </is>
       </c>
-      <c r="H27" s="4" t="n">
+      <c r="H27" s="6" t="n">
         <v>64.69</v>
       </c>
       <c r="I27" s="3" t="inlineStr">
@@ -2204,10 +2257,10 @@
           <t>3,00 %</t>
         </is>
       </c>
-      <c r="J27" s="4" t="n">
+      <c r="J27" s="6" t="n">
         <v>1.94</v>
       </c>
-      <c r="K27" s="4" t="n">
+      <c r="K27" s="6" t="n">
         <v>0</v>
       </c>
       <c r="L27" s="3" t="inlineStr">
@@ -2232,8 +2285,10 @@
           <t>202200000000027</t>
         </is>
       </c>
-      <c r="B28" s="4" t="n">
-        <v>4012022</v>
+      <c r="B28" s="4" t="inlineStr">
+        <is>
+          <t>04/01/2022</t>
+        </is>
       </c>
       <c r="C28" s="5" t="inlineStr">
         <is>
@@ -2260,7 +2315,7 @@
           <t>70,00</t>
         </is>
       </c>
-      <c r="H28" s="4" t="n">
+      <c r="H28" s="6" t="n">
         <v>70</v>
       </c>
       <c r="I28" s="3" t="inlineStr">
@@ -2268,10 +2323,10 @@
           <t>3,00 %</t>
         </is>
       </c>
-      <c r="J28" s="4" t="n">
+      <c r="J28" s="6" t="n">
         <v>2.1</v>
       </c>
-      <c r="K28" s="4" t="n">
+      <c r="K28" s="6" t="n">
         <v>0</v>
       </c>
       <c r="L28" s="3" t="inlineStr">
@@ -2296,8 +2351,10 @@
           <t>202200000000028</t>
         </is>
       </c>
-      <c r="B29" s="4" t="n">
-        <v>4012022</v>
+      <c r="B29" s="4" t="inlineStr">
+        <is>
+          <t>04/01/2022</t>
+        </is>
       </c>
       <c r="C29" s="5" t="inlineStr">
         <is>
@@ -2324,7 +2381,7 @@
           <t>700,00</t>
         </is>
       </c>
-      <c r="H29" s="4" t="n">
+      <c r="H29" s="6" t="n">
         <v>700</v>
       </c>
       <c r="I29" s="3" t="inlineStr">
@@ -2332,10 +2389,10 @@
           <t>3,00 %</t>
         </is>
       </c>
-      <c r="J29" s="4" t="n">
+      <c r="J29" s="6" t="n">
         <v>21</v>
       </c>
-      <c r="K29" s="4" t="n">
+      <c r="K29" s="6" t="n">
         <v>0</v>
       </c>
       <c r="L29" s="3" t="inlineStr">
@@ -2360,8 +2417,10 @@
           <t>202200000000029</t>
         </is>
       </c>
-      <c r="B30" s="4" t="n">
-        <v>4012022</v>
+      <c r="B30" s="4" t="inlineStr">
+        <is>
+          <t>04/01/2022</t>
+        </is>
       </c>
       <c r="C30" s="5" t="inlineStr">
         <is>
@@ -2388,7 +2447,7 @@
           <t>470,00</t>
         </is>
       </c>
-      <c r="H30" s="4" t="n">
+      <c r="H30" s="6" t="n">
         <v>470</v>
       </c>
       <c r="I30" s="3" t="inlineStr">
@@ -2396,10 +2455,10 @@
           <t>3,00 %</t>
         </is>
       </c>
-      <c r="J30" s="4" t="n">
+      <c r="J30" s="6" t="n">
         <v>14.1</v>
       </c>
-      <c r="K30" s="4" t="n">
+      <c r="K30" s="6" t="n">
         <v>0</v>
       </c>
       <c r="L30" s="3" t="inlineStr">
@@ -2424,8 +2483,10 @@
           <t>202200000000030</t>
         </is>
       </c>
-      <c r="B31" s="4" t="n">
-        <v>5012022</v>
+      <c r="B31" s="4" t="inlineStr">
+        <is>
+          <t>05/01/2022</t>
+        </is>
       </c>
       <c r="C31" s="5" t="inlineStr">
         <is>
@@ -2452,7 +2513,7 @@
           <t>34.808,08</t>
         </is>
       </c>
-      <c r="H31" s="4" t="n">
+      <c r="H31" s="6" t="n">
         <v>34808.08</v>
       </c>
       <c r="I31" s="3" t="inlineStr">
@@ -2460,10 +2521,10 @@
           <t>3,00 %</t>
         </is>
       </c>
-      <c r="J31" s="4" t="n">
+      <c r="J31" s="6" t="n">
         <v>1044.24</v>
       </c>
-      <c r="K31" s="4" t="n">
+      <c r="K31" s="6" t="n">
         <v>0</v>
       </c>
       <c r="L31" s="3" t="inlineStr">
@@ -2488,8 +2549,10 @@
           <t>202200000000031</t>
         </is>
       </c>
-      <c r="B32" s="4" t="n">
-        <v>5012022</v>
+      <c r="B32" s="4" t="inlineStr">
+        <is>
+          <t>05/01/2022</t>
+        </is>
       </c>
       <c r="C32" s="5" t="inlineStr">
         <is>
@@ -2516,7 +2579,7 @@
           <t>4.500,00</t>
         </is>
       </c>
-      <c r="H32" s="4" t="n">
+      <c r="H32" s="6" t="n">
         <v>4500</v>
       </c>
       <c r="I32" s="3" t="inlineStr">
@@ -2524,10 +2587,10 @@
           <t>3,00 %</t>
         </is>
       </c>
-      <c r="J32" s="4" t="n">
+      <c r="J32" s="6" t="n">
         <v>135</v>
       </c>
-      <c r="K32" s="4" t="n">
+      <c r="K32" s="6" t="n">
         <v>0</v>
       </c>
       <c r="L32" s="3" t="inlineStr">
@@ -2552,8 +2615,10 @@
           <t>202200000000032</t>
         </is>
       </c>
-      <c r="B33" s="4" t="n">
-        <v>5012022</v>
+      <c r="B33" s="4" t="inlineStr">
+        <is>
+          <t>05/01/2022</t>
+        </is>
       </c>
       <c r="C33" s="5" t="inlineStr">
         <is>
@@ -2580,7 +2645,7 @@
           <t>20,00</t>
         </is>
       </c>
-      <c r="H33" s="4" t="n">
+      <c r="H33" s="6" t="n">
         <v>20</v>
       </c>
       <c r="I33" s="3" t="inlineStr">
@@ -2588,10 +2653,10 @@
           <t>3,00 %</t>
         </is>
       </c>
-      <c r="J33" s="4" t="n">
+      <c r="J33" s="6" t="n">
         <v>0.6</v>
       </c>
-      <c r="K33" s="4" t="n">
+      <c r="K33" s="6" t="n">
         <v>0</v>
       </c>
       <c r="L33" s="3" t="inlineStr">
@@ -2616,8 +2681,10 @@
           <t>202200000000033</t>
         </is>
       </c>
-      <c r="B34" s="4" t="n">
-        <v>5012022</v>
+      <c r="B34" s="4" t="inlineStr">
+        <is>
+          <t>05/01/2022</t>
+        </is>
       </c>
       <c r="C34" s="5" t="inlineStr">
         <is>
@@ -2644,7 +2711,7 @@
           <t>632,97</t>
         </is>
       </c>
-      <c r="H34" s="4" t="n">
+      <c r="H34" s="6" t="n">
         <v>632.97</v>
       </c>
       <c r="I34" s="3" t="inlineStr">
@@ -2652,10 +2719,10 @@
           <t>3,00 %</t>
         </is>
       </c>
-      <c r="J34" s="4" t="n">
+      <c r="J34" s="6" t="n">
         <v>18.99</v>
       </c>
-      <c r="K34" s="4" t="n">
+      <c r="K34" s="6" t="n">
         <v>0</v>
       </c>
       <c r="L34" s="3" t="inlineStr">

</xml_diff>